<commit_message>
upload_file route and related functions refactored
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/generic_operator_feedback_v001.xlsx
+++ b/feedback_forms/current_versions/generic_operator_feedback_v001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one_drive\OneDriveLinks\RD Satellite Project - Operator Notification Materials for Review\spreadsheets\xl_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9BEC2A-5B24-4506-B6B2-CA03563CEC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1A6D34-875E-4A39-936F-61FACB53EE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="333" windowWidth="21293" windowHeight="13840" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="6160" yWindow="287" windowWidth="18053" windowHeight="13840" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="209">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -216,9 +216,6 @@
     </r>
   </si>
   <si>
-    <t>Facility ID</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -355,9 +352,6 @@
     </r>
   </si>
   <si>
-    <t>Q8 Answer.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -394,9 +388,6 @@
       </rPr>
       <t xml:space="preserve">  If applicable, please describe any events or activities that may have contributed to the plume observed on the date provided in Section 2.</t>
     </r>
-  </si>
-  <si>
-    <t>Q10 Answer.</t>
   </si>
   <si>
     <r>
@@ -2602,7 +2593,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:AG63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2897,9 +2890,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="25"/>
-      <c r="D23" s="55">
-        <v>153</v>
-      </c>
+      <c r="D23" s="55"/>
       <c r="E23" s="50"/>
       <c r="G23" s="26"/>
     </row>
@@ -2908,9 +2899,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="25"/>
-      <c r="D24" s="55">
-        <v>447</v>
-      </c>
+      <c r="D24" s="55"/>
       <c r="E24" s="25"/>
     </row>
     <row r="25" spans="2:33" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.5">
@@ -2918,9 +2907,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="25"/>
-      <c r="D25" s="56">
-        <v>45468</v>
-      </c>
+      <c r="D25" s="56"/>
       <c r="E25" s="25"/>
     </row>
     <row r="26" spans="2:33" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
@@ -2928,9 +2915,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="25"/>
-      <c r="D26" s="55">
-        <v>35.321100000000001</v>
-      </c>
+      <c r="D26" s="55"/>
       <c r="E26" s="50"/>
       <c r="G26" s="26"/>
     </row>
@@ -2939,9 +2924,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="25"/>
-      <c r="D27" s="55">
-        <v>-119.5808</v>
-      </c>
+      <c r="D27" s="55"/>
       <c r="E27" s="50"/>
       <c r="G27" s="26"/>
     </row>
@@ -2950,9 +2933,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="25"/>
-      <c r="D28" s="57" t="s">
-        <v>20</v>
-      </c>
+      <c r="D28" s="57"/>
       <c r="E28" s="50"/>
       <c r="F28" s="44"/>
       <c r="G28" s="26"/>
@@ -3006,9 +2987,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="44"/>
-      <c r="D32" s="45" t="s">
-        <v>22</v>
-      </c>
+      <c r="D32" s="45"/>
       <c r="E32" s="47"/>
       <c r="G32" s="26"/>
     </row>
@@ -3017,42 +2996,34 @@
         <v>23</v>
       </c>
       <c r="C33" s="47"/>
-      <c r="D33" s="45" t="s">
-        <v>24</v>
-      </c>
+      <c r="D33" s="45"/>
       <c r="E33" s="47"/>
       <c r="G33" s="26"/>
     </row>
     <row r="34" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B34" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="44"/>
-      <c r="D34" s="45" t="s">
-        <v>26</v>
-      </c>
+      <c r="D34" s="45"/>
       <c r="E34" s="47"/>
       <c r="G34" s="26"/>
     </row>
     <row r="35" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B35" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="44"/>
-      <c r="D35" s="45" t="s">
-        <v>28</v>
-      </c>
+      <c r="D35" s="45"/>
       <c r="E35" s="47"/>
       <c r="G35" s="26"/>
     </row>
     <row r="36" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B36" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="44"/>
-      <c r="D36" s="45" t="s">
-        <v>30</v>
-      </c>
+      <c r="D36" s="45"/>
       <c r="E36" s="47"/>
       <c r="G36" s="26"/>
     </row>
@@ -3102,38 +3073,34 @@
     </row>
     <row r="40" spans="2:33" s="10" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="47"/>
       <c r="D40" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G40" s="26"/>
     </row>
     <row r="41" spans="2:33" s="10" customFormat="1" ht="30.7" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B41" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="44"/>
-      <c r="D41" s="58">
-        <v>45152</v>
-      </c>
+      <c r="D41" s="58"/>
       <c r="E41" s="27"/>
       <c r="G41" s="26"/>
     </row>
     <row r="42" spans="2:33" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
       <c r="B42" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="47"/>
-      <c r="D42" s="45" t="s">
-        <v>35</v>
-      </c>
+      <c r="D42" s="45"/>
       <c r="G42" s="26"/>
     </row>
     <row r="43" spans="2:33" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B43" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C43" s="47"/>
       <c r="D43" s="45"/>
@@ -3141,12 +3108,10 @@
     </row>
     <row r="44" spans="2:33" s="10" customFormat="1" ht="45.35" x14ac:dyDescent="0.5">
       <c r="B44" s="28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C44" s="47"/>
-      <c r="D44" s="45" t="s">
-        <v>38</v>
-      </c>
+      <c r="D44" s="45"/>
       <c r="G44" s="26"/>
     </row>
     <row r="45" spans="2:33" s="20" customFormat="1" x14ac:dyDescent="0.5">
@@ -3196,11 +3161,9 @@
     </row>
     <row r="48" spans="2:33" s="20" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B48" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="45">
-        <v>500</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D48" s="45"/>
       <c r="G48" s="26"/>
       <c r="AG48" s="20" t="s">
         <v>0</v>
@@ -3208,29 +3171,25 @@
     </row>
     <row r="49" spans="2:33" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B49" s="36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C49" s="20"/>
-      <c r="D49" s="45">
-        <v>35.321100000000001</v>
-      </c>
+      <c r="D49" s="45"/>
       <c r="E49" s="20"/>
       <c r="G49" s="26"/>
     </row>
     <row r="50" spans="2:33" s="10" customFormat="1" ht="30.35" x14ac:dyDescent="0.5">
       <c r="B50" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C50" s="20"/>
-      <c r="D50" s="45">
-        <v>-119.5808</v>
-      </c>
+      <c r="D50" s="45"/>
       <c r="E50" s="20"/>
       <c r="G50" s="26"/>
     </row>
     <row r="51" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B51" s="46" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C51" s="20"/>
       <c r="D51" s="45"/>
@@ -3239,7 +3198,7 @@
     </row>
     <row r="52" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B52" s="44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="45"/>
@@ -3292,36 +3251,30 @@
     </row>
     <row r="56" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B56" s="44" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D56" s="45"/>
       <c r="G56" s="26"/>
     </row>
     <row r="57" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B57" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D57" s="58">
-        <v>45275</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D57" s="58"/>
       <c r="G57" s="26"/>
     </row>
     <row r="58" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B58" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="58">
-        <v>85</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D58" s="58"/>
       <c r="G58" s="26"/>
     </row>
     <row r="59" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B59" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D59" s="45">
-        <v>85</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D59" s="45"/>
       <c r="G59" s="26"/>
     </row>
     <row r="60" spans="2:33" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.5">
@@ -3334,12 +3287,10 @@
     <row r="62" spans="2:33" s="30" customFormat="1" x14ac:dyDescent="0.5"/>
     <row r="63" spans="2:33" s="10" customFormat="1" ht="15.35" x14ac:dyDescent="0.5">
       <c r="B63" s="28" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C63" s="31"/>
-      <c r="D63" s="45" t="s">
-        <v>49</v>
-      </c>
+      <c r="D63" s="45"/>
       <c r="G63" s="26"/>
     </row>
   </sheetData>
@@ -3386,7 +3337,7 @@
   <sheetData>
     <row r="2" spans="1:18" s="11" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="12"/>
       <c r="F2" s="12"/>
@@ -3408,15 +3359,15 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B7" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.5">
@@ -3424,18 +3375,18 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B10" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" s="14"/>
       <c r="F10" s="13"/>
@@ -3443,10 +3394,10 @@
     </row>
     <row r="11" spans="1:18" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B11" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D11" s="14"/>
       <c r="F11" s="13"/>
@@ -3454,10 +3405,10 @@
     </row>
     <row r="12" spans="1:18" s="10" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="B12" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" s="14"/>
       <c r="F12" s="13"/>
@@ -3465,10 +3416,10 @@
     </row>
     <row r="13" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B13" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="14"/>
       <c r="F13" s="13"/>
@@ -3484,7 +3435,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="B16" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
@@ -3515,22 +3466,22 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -4492,15 +4443,15 @@
   <sheetData>
     <row r="2" spans="1:17" s="39" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="39" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
@@ -4517,10 +4468,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
@@ -4536,10 +4487,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
@@ -4581,27 +4532,27 @@
     </row>
     <row r="10" spans="1:17" s="40" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B10" s="40" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B12" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B17" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.5">
@@ -4609,42 +4560,42 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B23" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.5">
@@ -4652,7 +4603,7 @@
     </row>
     <row r="31" spans="2:7" s="40" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B31" s="40" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.5">
@@ -4660,10 +4611,10 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B33" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G33"/>
     </row>
@@ -4674,7 +4625,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="str" cm="1">
         <f t="array" ref="C35:C38">_xlfn._xlws.FILTER($B$35:$B$38,$B$35:$B$38 &lt;&gt; "")</f>
@@ -4740,55 +4691,55 @@
   <sheetData>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B14" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -4813,39 +4764,39 @@
   <sheetData>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
@@ -4855,26 +4806,26 @@
     <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="1:3" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B14" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4904,17 +4855,17 @@
   <sheetData>
     <row r="2" spans="1:6" s="11" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C2" s="12"/>
       <c r="F2" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="9"/>
@@ -4940,285 +4891,285 @@
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B10" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
         <v>116</v>
       </c>
-      <c r="C12" t="s">
-        <v>119</v>
-      </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -5229,30 +5180,30 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -5263,13 +5214,13 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -5280,13 +5231,13 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D30" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -5297,47 +5248,47 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -5348,13 +5299,13 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -5365,30 +5316,30 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B36" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -5399,13 +5350,13 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -5416,13 +5367,13 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D38" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -5433,13 +5384,13 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -5450,13 +5401,13 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B40" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D40" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -5467,13 +5418,13 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D41" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -5484,30 +5435,30 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D42" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -5518,13 +5469,13 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -5535,47 +5486,47 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D46" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -5586,13 +5537,13 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.5">
       <c r="B48" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D48" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -5637,47 +5588,47 @@
   <sheetData>
     <row r="2" spans="2:13" s="11" customFormat="1" ht="20.7" x14ac:dyDescent="0.7">
       <c r="B2" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C2" s="12"/>
       <c r="F2" s="15"/>
     </row>
     <row r="6" spans="2:13" ht="86" x14ac:dyDescent="0.5">
       <c r="B6" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="F6" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="G6" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="H6" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="I6" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="J6" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="K6" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="L6" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="M6" s="41" t="s">
         <v>207</v>
-      </c>
-      <c r="K6" s="41" t="s">
-        <v>208</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="M6" s="41" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.5">
@@ -5966,26 +5917,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -6220,26 +6151,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC83B422-5B73-4269-9006-1DDE9C149499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6258,6 +6190,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" enabled="0" method="" siteId="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" removed="1"/>

</xml_diff>

<commit_message>
trying to get staged import to work
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/generic_operator_feedback_v001.xlsx
+++ b/feedback_forms/current_versions/generic_operator_feedback_v001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1A6D34-875E-4A39-936F-61FACB53EE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B780F7EB-1834-405E-A49B-B5C7A505D59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6160" yWindow="287" windowWidth="18053" windowHeight="13840" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
@@ -2593,8 +2593,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:AG63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>